<commit_message>
Changes to Observation and Patient to pass validator
</commit_message>
<xml_diff>
--- a/docs/CareConnect-ACVPU-Observation-1.xlsx
+++ b/docs/CareConnect-ACVPU-Observation-1.xlsx
@@ -1979,13 +1979,13 @@
     <col min="2" max="2" width="22.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.63671875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.6328125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1996,22 +1996,22 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="171.48046875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="67.76953125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="72.328125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="242.6875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="22.03125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Added ConditionEpisodicity ConceptMap. #2
</commit_message>
<xml_diff>
--- a/docs/CareConnect-ACVPU-Observation-1.xlsx
+++ b/docs/CareConnect-ACVPU-Observation-1.xlsx
@@ -1979,13 +1979,13 @@
     <col min="2" max="2" width="22.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.63671875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.6328125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1996,22 +1996,22 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="171.48046875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="67.76953125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="72.328125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="242.6875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="22.03125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Fixed trailing space in DocumentReference profile and incorrect binding in Obs-ACVPU profile
</commit_message>
<xml_diff>
--- a/docs/CareConnect-ACVPU-Observation-1.xlsx
+++ b/docs/CareConnect-ACVPU-Observation-1.xlsx
@@ -698,10 +698,13 @@
     <t>Knowing what kind of observation is being made is essential to understanding the observation.</t>
   </si>
   <si>
-    <t>A code from SNOMED Clinical Terminology UK</t>
-  </si>
-  <si>
-    <t>http://snomed.info/sct</t>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Codes identifying names of simple observations.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
   </si>
   <si>
     <t>Event.code</t>
@@ -775,6 +778,9 @@
   </si>
   <si>
     <t>Need to be unambiguous about the source of the definition of the symbol.</t>
+  </si>
+  <si>
+    <t>http://snomed.info/sct</t>
   </si>
   <si>
     <t>Coding.system</t>
@@ -1244,9 +1250,6 @@
     <t>Only used if not implicit in code found in Observation.code.  In many systems, this may be represented as a related observation instead of an inline component.   If the use case requires BodySite to be handled as a separate resource (e.g. to identify and track separately) then use the standard extension[ body-site-instance](http://hl7.org/fhir/STU3/extension-body-site-instance.html).</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
     <t>Codes describing anatomical locations. May include laterality.</t>
   </si>
   <si>
@@ -1364,6 +1367,9 @@
   </si>
   <si>
     <t>Observation.method.coding</t>
+  </si>
+  <si>
+    <t>A code from SNOMED Clinical Terminology UK</t>
   </si>
   <si>
     <t>https://fhir.hl7.org.uk/STU3/ValueSet/CareConnect-ObservationMethod-1</t>
@@ -1728,12 +1734,6 @@
   </si>
   <si>
     <t>Describes what was observed. Sometimes this is called the observation "code".</t>
-  </si>
-  <si>
-    <t>Codes identifying names of simple observations.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
   </si>
   <si>
     <t>&lt; 363787002 |Observable entity| OR @@ -4662,13 +4662,13 @@
         <v>45</v>
       </c>
       <c r="W23" t="s" s="2">
-        <v>136</v>
+        <v>219</v>
       </c>
       <c r="X23" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="Y23" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="Z23" t="s" s="2">
         <v>45</v>
@@ -4701,27 +4701,27 @@
         <v>45</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4836,7 +4836,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4953,7 +4953,7 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4976,19 +4976,19 @@
         <v>57</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -5037,7 +5037,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -5058,10 +5058,10 @@
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
@@ -5072,7 +5072,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -5187,7 +5187,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -5304,7 +5304,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -5330,23 +5330,23 @@
         <v>69</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P29" s="2"/>
       <c r="Q29" t="s" s="2">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="R29" t="s" s="2">
         <v>45</v>
@@ -5388,7 +5388,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -5409,10 +5409,10 @@
         <v>45</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
@@ -5423,7 +5423,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -5449,13 +5449,13 @@
         <v>120</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5505,7 +5505,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5526,10 +5526,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5540,7 +5540,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5566,21 +5566,21 @@
         <v>75</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="O31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P31" s="2"/>
       <c r="Q31" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="R31" t="s" s="2">
         <v>45</v>
@@ -5622,7 +5622,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5643,10 +5643,10 @@
         <v>45</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
@@ -5657,7 +5657,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5683,21 +5683,21 @@
         <v>120</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="R32" t="s" s="2">
         <v>45</v>
@@ -5739,7 +5739,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5760,10 +5760,10 @@
         <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5774,7 +5774,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5797,19 +5797,19 @@
         <v>57</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5858,7 +5858,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5879,10 +5879,10 @@
         <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5893,7 +5893,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5919,16 +5919,16 @@
         <v>120</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="O34" t="s" s="2">
         <v>45</v>
@@ -5977,7 +5977,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5998,10 +5998,10 @@
         <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -6012,7 +6012,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -6035,19 +6035,19 @@
         <v>57</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
@@ -6096,7 +6096,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -6111,19 +6111,19 @@
         <v>45</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>45</v>
@@ -6131,11 +6131,11 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -6154,19 +6154,19 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
@@ -6215,7 +6215,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -6230,19 +6230,19 @@
         <v>45</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>45</v>
@@ -6250,11 +6250,11 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
@@ -6273,19 +6273,19 @@
         <v>57</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -6334,7 +6334,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -6349,19 +6349,19 @@
         <v>45</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>45</v>
@@ -6369,7 +6369,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6392,16 +6392,16 @@
         <v>57</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
@@ -6451,7 +6451,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -6472,13 +6472,13 @@
         <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>45</v>
@@ -6486,7 +6486,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6509,17 +6509,17 @@
         <v>57</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6568,7 +6568,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6583,19 +6583,19 @@
         <v>45</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>45</v>
@@ -6603,7 +6603,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6629,16 +6629,16 @@
         <v>142</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6675,17 +6675,17 @@
         <v>45</v>
       </c>
       <c r="AA40" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="AB40" s="2"/>
       <c r="AC40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD40" t="s" s="2">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6694,36 +6694,36 @@
         <v>56</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C41" t="s" s="2">
         <v>45</v>
@@ -6748,16 +6748,16 @@
         <v>142</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6785,63 +6785,63 @@
         <v>136</v>
       </c>
       <c r="X41" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE41" t="s" s="2">
+        <v>339</v>
+      </c>
+      <c r="AF41" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG41" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="AL41" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="AM41" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="AN41" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO41" t="s" s="2">
         <v>351</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA41" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC41" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD41" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE41" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="AF41" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG41" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH41" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="AI41" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>347</v>
-      </c>
-      <c r="AM41" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="AN41" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO41" t="s" s="2">
-        <v>349</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6956,7 +6956,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -7073,7 +7073,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -7096,19 +7096,19 @@
         <v>57</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -7157,7 +7157,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -7178,10 +7178,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -7192,7 +7192,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -7307,7 +7307,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7424,7 +7424,7 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7450,23 +7450,23 @@
         <v>69</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P47" s="2"/>
       <c r="Q47" t="s" s="2">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="R47" t="s" s="2">
         <v>45</v>
@@ -7508,7 +7508,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7529,10 +7529,10 @@
         <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7543,7 +7543,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7569,13 +7569,13 @@
         <v>120</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
@@ -7625,7 +7625,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
@@ -7646,10 +7646,10 @@
         <v>45</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7660,7 +7660,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7686,14 +7686,14 @@
         <v>75</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7742,7 +7742,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7763,10 +7763,10 @@
         <v>45</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7777,7 +7777,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7803,14 +7803,14 @@
         <v>120</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7859,7 +7859,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7880,10 +7880,10 @@
         <v>45</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
@@ -7894,7 +7894,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7917,19 +7917,19 @@
         <v>57</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7978,7 +7978,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7999,10 +7999,10 @@
         <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
@@ -8013,7 +8013,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -8039,16 +8039,16 @@
         <v>120</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -8097,7 +8097,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -8118,10 +8118,10 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
@@ -8132,7 +8132,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -8158,16 +8158,16 @@
         <v>142</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -8195,10 +8195,10 @@
         <v>79</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -8216,7 +8216,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -8225,13 +8225,13 @@
         <v>56</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="AI53" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="AK53" t="s" s="2">
         <v>45</v>
@@ -8240,7 +8240,7 @@
         <v>99</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
@@ -8251,11 +8251,11 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" t="s" s="2">
@@ -8277,14 +8277,14 @@
         <v>142</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" t="s" s="2">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>45</v>
@@ -8312,10 +8312,10 @@
         <v>79</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>45</v>
@@ -8333,7 +8333,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -8351,24 +8351,24 @@
         <v>45</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO54" t="s" s="2">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8394,14 +8394,14 @@
         <v>120</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>45</v>
@@ -8450,7 +8450,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8465,16 +8465,16 @@
         <v>45</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>45</v>
@@ -8485,7 +8485,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8511,13 +8511,13 @@
         <v>142</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
@@ -8543,13 +8543,13 @@
         <v>45</v>
       </c>
       <c r="W56" t="s" s="2">
-        <v>395</v>
+        <v>219</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="Z56" t="s" s="2">
         <v>45</v>
@@ -8567,7 +8567,7 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
@@ -8585,24 +8585,24 @@
         <v>45</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO56" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -8717,7 +8717,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8834,7 +8834,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8857,19 +8857,19 @@
         <v>57</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>45</v>
@@ -8906,7 +8906,7 @@
         <v>45</v>
       </c>
       <c r="AA59" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AB59" s="2"/>
       <c r="AC59" t="s" s="2">
@@ -8916,7 +8916,7 @@
         <v>129</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
@@ -8937,10 +8937,10 @@
         <v>45</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>45</v>
@@ -8951,10 +8951,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C60" t="s" s="2">
         <v>45</v>
@@ -8976,19 +8976,19 @@
         <v>57</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>45</v>
@@ -9016,10 +9016,10 @@
         <v>209</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>45</v>
@@ -9037,7 +9037,7 @@
         <v>45</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -9058,10 +9058,10 @@
         <v>45</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>45</v>
@@ -9072,7 +9072,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -9187,7 +9187,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -9213,10 +9213,10 @@
         <v>102</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -9302,10 +9302,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C63" t="s" s="2">
         <v>45</v>
@@ -9327,13 +9327,13 @@
         <v>45</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -9419,7 +9419,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9445,23 +9445,23 @@
         <v>69</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O64" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P64" s="2"/>
       <c r="Q64" t="s" s="2">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="R64" t="s" s="2">
         <v>45</v>
@@ -9503,7 +9503,7 @@
         <v>45</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>43</v>
@@ -9524,10 +9524,10 @@
         <v>45</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>45</v>
@@ -9538,7 +9538,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9564,13 +9564,13 @@
         <v>120</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
@@ -9620,7 +9620,7 @@
         <v>45</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>43</v>
@@ -9641,10 +9641,10 @@
         <v>45</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="AN65" t="s" s="2">
         <v>45</v>
@@ -9655,7 +9655,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9681,14 +9681,14 @@
         <v>75</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="O66" t="s" s="2">
         <v>45</v>
@@ -9737,7 +9737,7 @@
         <v>45</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>43</v>
@@ -9758,10 +9758,10 @@
         <v>45</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AN66" t="s" s="2">
         <v>45</v>
@@ -9772,7 +9772,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9798,14 +9798,14 @@
         <v>120</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="O67" t="s" s="2">
         <v>45</v>
@@ -9854,7 +9854,7 @@
         <v>45</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>43</v>
@@ -9875,10 +9875,10 @@
         <v>45</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>45</v>
@@ -9889,7 +9889,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9912,19 +9912,19 @@
         <v>57</v>
       </c>
       <c r="J68" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="N68" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>45</v>
@@ -9973,7 +9973,7 @@
         <v>45</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>43</v>
@@ -9994,10 +9994,10 @@
         <v>45</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>45</v>
@@ -10008,7 +10008,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -10034,16 +10034,16 @@
         <v>120</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>45</v>
@@ -10092,7 +10092,7 @@
         <v>45</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>43</v>
@@ -10113,10 +10113,10 @@
         <v>45</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>45</v>
@@ -10127,7 +10127,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -10153,16 +10153,16 @@
         <v>142</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>45</v>
@@ -10187,13 +10187,13 @@
         <v>45</v>
       </c>
       <c r="W70" t="s" s="2">
-        <v>395</v>
+        <v>219</v>
       </c>
       <c r="X70" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="Y70" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="Z70" t="s" s="2">
         <v>45</v>
@@ -10211,7 +10211,7 @@
         <v>45</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>43</v>
@@ -10232,10 +10232,10 @@
         <v>45</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="AN70" t="s" s="2">
         <v>45</v>
@@ -10246,7 +10246,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -10361,7 +10361,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -10478,7 +10478,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -10501,19 +10501,19 @@
         <v>57</v>
       </c>
       <c r="J73" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N73" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>45</v>
@@ -10550,7 +10550,7 @@
         <v>45</v>
       </c>
       <c r="AA73" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AB73" s="2"/>
       <c r="AC73" t="s" s="2">
@@ -10560,7 +10560,7 @@
         <v>129</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>43</v>
@@ -10581,10 +10581,10 @@
         <v>45</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AN73" t="s" s="2">
         <v>45</v>
@@ -10595,10 +10595,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C74" t="s" s="2">
         <v>45</v>
@@ -10620,19 +10620,19 @@
         <v>57</v>
       </c>
       <c r="J74" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N74" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O74" t="s" s="2">
         <v>45</v>
@@ -10660,10 +10660,10 @@
         <v>209</v>
       </c>
       <c r="X74" t="s" s="2">
-        <v>219</v>
+        <v>436</v>
       </c>
       <c r="Y74" t="s" s="2">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="Z74" t="s" s="2">
         <v>45</v>
@@ -10681,7 +10681,7 @@
         <v>45</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF74" t="s" s="2">
         <v>43</v>
@@ -10702,10 +10702,10 @@
         <v>45</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AN74" t="s" s="2">
         <v>45</v>
@@ -10716,7 +10716,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -10831,7 +10831,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -10857,10 +10857,10 @@
         <v>102</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -10946,10 +10946,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C77" t="s" s="2">
         <v>45</v>
@@ -10971,13 +10971,13 @@
         <v>45</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -11063,7 +11063,7 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
@@ -11089,23 +11089,23 @@
         <v>69</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O78" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P78" s="2"/>
       <c r="Q78" t="s" s="2">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="R78" t="s" s="2">
         <v>45</v>
@@ -11147,7 +11147,7 @@
         <v>45</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>43</v>
@@ -11168,10 +11168,10 @@
         <v>45</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AN78" t="s" s="2">
         <v>45</v>
@@ -11182,7 +11182,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -11208,13 +11208,13 @@
         <v>120</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" t="s" s="2">
@@ -11264,7 +11264,7 @@
         <v>45</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>43</v>
@@ -11285,10 +11285,10 @@
         <v>45</v>
       </c>
       <c r="AL79" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="AN79" t="s" s="2">
         <v>45</v>
@@ -11299,7 +11299,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -11325,14 +11325,14 @@
         <v>75</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="O80" t="s" s="2">
         <v>45</v>
@@ -11381,7 +11381,7 @@
         <v>45</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>43</v>
@@ -11402,10 +11402,10 @@
         <v>45</v>
       </c>
       <c r="AL80" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AN80" t="s" s="2">
         <v>45</v>
@@ -11416,7 +11416,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -11442,14 +11442,14 @@
         <v>120</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="M81" s="2"/>
       <c r="N81" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="O81" t="s" s="2">
         <v>45</v>
@@ -11498,7 +11498,7 @@
         <v>45</v>
       </c>
       <c r="AE81" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AF81" t="s" s="2">
         <v>43</v>
@@ -11519,10 +11519,10 @@
         <v>45</v>
       </c>
       <c r="AL81" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="AM81" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AN81" t="s" s="2">
         <v>45</v>
@@ -11533,7 +11533,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -11556,19 +11556,19 @@
         <v>57</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="N82" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="O82" t="s" s="2">
         <v>45</v>
@@ -11617,7 +11617,7 @@
         <v>45</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>43</v>
@@ -11638,10 +11638,10 @@
         <v>45</v>
       </c>
       <c r="AL82" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AN82" t="s" s="2">
         <v>45</v>
@@ -11652,7 +11652,7 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
@@ -11678,16 +11678,16 @@
         <v>120</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="N83" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>45</v>
@@ -11736,7 +11736,7 @@
         <v>45</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>43</v>
@@ -11757,10 +11757,10 @@
         <v>45</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AM83" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AN83" t="s" s="2">
         <v>45</v>
@@ -11771,7 +11771,7 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -11794,16 +11794,16 @@
         <v>45</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="N84" s="2"/>
       <c r="O84" t="s" s="2">
@@ -11853,7 +11853,7 @@
         <v>45</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>43</v>
@@ -11871,24 +11871,24 @@
         <v>45</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="AL84" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO84" t="s" s="2">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -11911,16 +11911,16 @@
         <v>45</v>
       </c>
       <c r="J85" t="s" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="N85" s="2"/>
       <c r="O85" t="s" s="2">
@@ -11970,7 +11970,7 @@
         <v>45</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>43</v>
@@ -11988,24 +11988,24 @@
         <v>45</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="AM85" t="s" s="2">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="AN85" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO85" t="s" s="2">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -12028,19 +12028,19 @@
         <v>45</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="N86" t="s" s="2">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>45</v>
@@ -12089,7 +12089,7 @@
         <v>45</v>
       </c>
       <c r="AE86" t="s" s="2">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="AF86" t="s" s="2">
         <v>43</v>
@@ -12101,7 +12101,7 @@
         <v>45</v>
       </c>
       <c r="AI86" t="s" s="2">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="AJ86" t="s" s="2">
         <v>45</v>
@@ -12110,10 +12110,10 @@
         <v>45</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="AN86" t="s" s="2">
         <v>45</v>
@@ -12124,7 +12124,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -12239,7 +12239,7 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -12356,11 +12356,11 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" t="s" s="2">
@@ -12385,7 +12385,7 @@
         <v>108</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="M89" t="s" s="2">
         <v>105</v>
@@ -12438,7 +12438,7 @@
         <v>45</v>
       </c>
       <c r="AE89" t="s" s="2">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="AF89" t="s" s="2">
         <v>43</v>
@@ -12473,7 +12473,7 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -12496,13 +12496,13 @@
         <v>45</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -12553,7 +12553,7 @@
         <v>45</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="AF90" t="s" s="2">
         <v>43</v>
@@ -12562,7 +12562,7 @@
         <v>56</v>
       </c>
       <c r="AH90" t="s" s="2">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="AI90" t="s" s="2">
         <v>45</v>
@@ -12574,10 +12574,10 @@
         <v>45</v>
       </c>
       <c r="AL90" t="s" s="2">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="AN90" t="s" s="2">
         <v>45</v>
@@ -12588,7 +12588,7 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -12611,13 +12611,13 @@
         <v>45</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
@@ -12668,31 +12668,31 @@
         <v>45</v>
       </c>
       <c r="AE91" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="AF91" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG91" t="s" s="2">
+        <v>56</v>
+      </c>
+      <c r="AH91" t="s" s="2">
+        <v>483</v>
+      </c>
+      <c r="AI91" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AJ91" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK91" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL91" t="s" s="2">
         <v>484</v>
       </c>
-      <c r="AF91" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG91" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="AH91" t="s" s="2">
-        <v>481</v>
-      </c>
-      <c r="AI91" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AJ91" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK91" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL91" t="s" s="2">
-        <v>482</v>
-      </c>
       <c r="AM91" t="s" s="2">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="AN91" t="s" s="2">
         <v>45</v>
@@ -12703,7 +12703,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -12729,16 +12729,16 @@
         <v>142</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="N92" t="s" s="2">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="O92" t="s" s="2">
         <v>45</v>
@@ -12766,10 +12766,10 @@
         <v>79</v>
       </c>
       <c r="X92" t="s" s="2">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="Y92" t="s" s="2">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="Z92" t="s" s="2">
         <v>45</v>
@@ -12787,7 +12787,7 @@
         <v>45</v>
       </c>
       <c r="AE92" t="s" s="2">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="AF92" t="s" s="2">
         <v>43</v>
@@ -12805,13 +12805,13 @@
         <v>45</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="AL92" t="s" s="2">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="AM92" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AN92" t="s" s="2">
         <v>45</v>
@@ -12822,7 +12822,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -12848,16 +12848,16 @@
         <v>142</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="M93" t="s" s="2">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="N93" t="s" s="2">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="O93" t="s" s="2">
         <v>45</v>
@@ -12882,13 +12882,13 @@
         <v>45</v>
       </c>
       <c r="W93" t="s" s="2">
-        <v>395</v>
+        <v>219</v>
       </c>
       <c r="X93" t="s" s="2">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="Y93" t="s" s="2">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="Z93" t="s" s="2">
         <v>45</v>
@@ -12906,7 +12906,7 @@
         <v>45</v>
       </c>
       <c r="AE93" t="s" s="2">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="AF93" t="s" s="2">
         <v>43</v>
@@ -12924,13 +12924,13 @@
         <v>45</v>
       </c>
       <c r="AK93" t="s" s="2">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="AL93" t="s" s="2">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="AM93" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AN93" t="s" s="2">
         <v>45</v>
@@ -12941,7 +12941,7 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
@@ -12964,17 +12964,17 @@
         <v>45</v>
       </c>
       <c r="J94" t="s" s="2">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="K94" t="s" s="2">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="L94" t="s" s="2">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="M94" s="2"/>
       <c r="N94" t="s" s="2">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="O94" t="s" s="2">
         <v>45</v>
@@ -13023,7 +13023,7 @@
         <v>45</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="AF94" t="s" s="2">
         <v>43</v>
@@ -13047,7 +13047,7 @@
         <v>45</v>
       </c>
       <c r="AM94" t="s" s="2">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="AN94" t="s" s="2">
         <v>45</v>
@@ -13058,7 +13058,7 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
@@ -13084,10 +13084,10 @@
         <v>120</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
@@ -13138,7 +13138,7 @@
         <v>45</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>43</v>
@@ -13159,10 +13159,10 @@
         <v>45</v>
       </c>
       <c r="AL95" t="s" s="2">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="AM95" t="s" s="2">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="AN95" t="s" s="2">
         <v>45</v>
@@ -13173,7 +13173,7 @@
     </row>
     <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s" s="2">
@@ -13196,19 +13196,19 @@
         <v>57</v>
       </c>
       <c r="J96" t="s" s="2">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="K96" t="s" s="2">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="M96" t="s" s="2">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="N96" t="s" s="2">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="O96" t="s" s="2">
         <v>45</v>
@@ -13257,7 +13257,7 @@
         <v>45</v>
       </c>
       <c r="AE96" t="s" s="2">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="AF96" t="s" s="2">
         <v>43</v>
@@ -13269,7 +13269,7 @@
         <v>45</v>
       </c>
       <c r="AI96" t="s" s="2">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="AJ96" t="s" s="2">
         <v>45</v>
@@ -13278,10 +13278,10 @@
         <v>45</v>
       </c>
       <c r="AL96" t="s" s="2">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="AM96" t="s" s="2">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="AN96" t="s" s="2">
         <v>45</v>
@@ -13292,7 +13292,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -13407,7 +13407,7 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
@@ -13524,11 +13524,11 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" t="s" s="2">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" t="s" s="2">
@@ -13553,7 +13553,7 @@
         <v>108</v>
       </c>
       <c r="L99" t="s" s="2">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="M99" t="s" s="2">
         <v>105</v>
@@ -13606,7 +13606,7 @@
         <v>45</v>
       </c>
       <c r="AE99" t="s" s="2">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="AF99" t="s" s="2">
         <v>43</v>
@@ -13641,7 +13641,7 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -13667,16 +13667,16 @@
         <v>75</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="M100" t="s" s="2">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="N100" t="s" s="2">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="O100" t="s" s="2">
         <v>45</v>
@@ -13704,10 +13704,10 @@
         <v>136</v>
       </c>
       <c r="X100" t="s" s="2">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="Y100" t="s" s="2">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="Z100" t="s" s="2">
         <v>45</v>
@@ -13725,7 +13725,7 @@
         <v>45</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>43</v>
@@ -13749,7 +13749,7 @@
         <v>99</v>
       </c>
       <c r="AM100" t="s" s="2">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="AN100" t="s" s="2">
         <v>45</v>
@@ -13760,7 +13760,7 @@
     </row>
     <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -13783,13 +13783,13 @@
         <v>45</v>
       </c>
       <c r="J101" t="s" s="2">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="K101" t="s" s="2">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="L101" t="s" s="2">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="M101" s="2"/>
       <c r="N101" s="2"/>
@@ -13840,7 +13840,7 @@
         <v>45</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>56</v>
@@ -13864,7 +13864,7 @@
         <v>45</v>
       </c>
       <c r="AM101" t="s" s="2">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="AN101" t="s" s="2">
         <v>45</v>
@@ -13875,7 +13875,7 @@
     </row>
     <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -13898,19 +13898,19 @@
         <v>57</v>
       </c>
       <c r="J102" t="s" s="2">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="N102" t="s" s="2">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="O102" t="s" s="2">
         <v>45</v>
@@ -13959,7 +13959,7 @@
         <v>45</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>43</v>
@@ -13971,7 +13971,7 @@
         <v>45</v>
       </c>
       <c r="AI102" t="s" s="2">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="AJ102" t="s" s="2">
         <v>45</v>
@@ -13980,10 +13980,10 @@
         <v>45</v>
       </c>
       <c r="AL102" t="s" s="2">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="AM102" t="s" s="2">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="AN102" t="s" s="2">
         <v>45</v>
@@ -13994,7 +13994,7 @@
     </row>
     <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -14109,7 +14109,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -14226,11 +14226,11 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" t="s" s="2">
@@ -14255,7 +14255,7 @@
         <v>108</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="M105" t="s" s="2">
         <v>105</v>
@@ -14308,7 +14308,7 @@
         <v>45</v>
       </c>
       <c r="AE105" t="s" s="2">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="AF105" t="s" s="2">
         <v>43</v>
@@ -14343,7 +14343,7 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -14369,10 +14369,10 @@
         <v>142</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="M106" s="2"/>
       <c r="N106" t="s" s="2">
@@ -14401,13 +14401,13 @@
         <v>45</v>
       </c>
       <c r="W106" t="s" s="2">
-        <v>395</v>
+        <v>219</v>
       </c>
       <c r="X106" t="s" s="2">
-        <v>551</v>
+        <v>220</v>
       </c>
       <c r="Y106" t="s" s="2">
-        <v>552</v>
+        <v>221</v>
       </c>
       <c r="Z106" t="s" s="2">
         <v>45</v>
@@ -14425,7 +14425,7 @@
         <v>45</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="AF106" t="s" s="2">
         <v>56</v>
@@ -14446,13 +14446,13 @@
         <v>553</v>
       </c>
       <c r="AL106" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AM106" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AN106" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AO106" t="s" s="2">
         <v>45</v>
@@ -14715,19 +14715,19 @@
         <v>57</v>
       </c>
       <c r="J109" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K109" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M109" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N109" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O109" t="s" s="2">
         <v>45</v>
@@ -14774,7 +14774,7 @@
         <v>129</v>
       </c>
       <c r="AE109" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF109" t="s" s="2">
         <v>43</v>
@@ -14795,10 +14795,10 @@
         <v>45</v>
       </c>
       <c r="AL109" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AM109" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AN109" t="s" s="2">
         <v>45</v>
@@ -14812,7 +14812,7 @@
         <v>556</v>
       </c>
       <c r="B110" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C110" t="s" s="2">
         <v>45</v>
@@ -14834,19 +14834,19 @@
         <v>57</v>
       </c>
       <c r="J110" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K110" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L110" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M110" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N110" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O110" t="s" s="2">
         <v>45</v>
@@ -14895,7 +14895,7 @@
         <v>45</v>
       </c>
       <c r="AE110" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="AF110" t="s" s="2">
         <v>43</v>
@@ -14916,10 +14916,10 @@
         <v>45</v>
       </c>
       <c r="AL110" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AM110" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AN110" t="s" s="2">
         <v>45</v>
@@ -15071,10 +15071,10 @@
         <v>102</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M112" s="2"/>
       <c r="N112" s="2"/>
@@ -15163,7 +15163,7 @@
         <v>561</v>
       </c>
       <c r="B113" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C113" t="s" s="2">
         <v>45</v>
@@ -15185,13 +15185,13 @@
         <v>45</v>
       </c>
       <c r="J113" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="M113" s="2"/>
       <c r="N113" s="2"/>
@@ -15303,23 +15303,23 @@
         <v>69</v>
       </c>
       <c r="K114" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L114" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M114" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N114" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O114" t="s" s="2">
         <v>45</v>
       </c>
       <c r="P114" s="2"/>
       <c r="Q114" t="s" s="2">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="R114" t="s" s="2">
         <v>45</v>
@@ -15361,7 +15361,7 @@
         <v>45</v>
       </c>
       <c r="AE114" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>43</v>
@@ -15382,10 +15382,10 @@
         <v>45</v>
       </c>
       <c r="AL114" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AM114" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AN114" t="s" s="2">
         <v>45</v>
@@ -15422,13 +15422,13 @@
         <v>120</v>
       </c>
       <c r="K115" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L115" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M115" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="N115" s="2"/>
       <c r="O115" t="s" s="2">
@@ -15478,7 +15478,7 @@
         <v>45</v>
       </c>
       <c r="AE115" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AF115" t="s" s="2">
         <v>43</v>
@@ -15499,10 +15499,10 @@
         <v>45</v>
       </c>
       <c r="AL115" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AM115" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="AN115" t="s" s="2">
         <v>45</v>
@@ -15539,14 +15539,14 @@
         <v>75</v>
       </c>
       <c r="K116" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="L116" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="M116" s="2"/>
       <c r="N116" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="O116" t="s" s="2">
         <v>45</v>
@@ -15595,7 +15595,7 @@
         <v>45</v>
       </c>
       <c r="AE116" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AF116" t="s" s="2">
         <v>43</v>
@@ -15616,10 +15616,10 @@
         <v>45</v>
       </c>
       <c r="AL116" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AM116" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AN116" t="s" s="2">
         <v>45</v>
@@ -15656,14 +15656,14 @@
         <v>120</v>
       </c>
       <c r="K117" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="L117" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="M117" s="2"/>
       <c r="N117" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="O117" t="s" s="2">
         <v>45</v>
@@ -15712,7 +15712,7 @@
         <v>45</v>
       </c>
       <c r="AE117" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AF117" t="s" s="2">
         <v>43</v>
@@ -15733,10 +15733,10 @@
         <v>45</v>
       </c>
       <c r="AL117" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="AM117" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AN117" t="s" s="2">
         <v>45</v>
@@ -15770,19 +15770,19 @@
         <v>57</v>
       </c>
       <c r="J118" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="K118" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="L118" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M118" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="N118" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="O118" t="s" s="2">
         <v>45</v>
@@ -15831,7 +15831,7 @@
         <v>45</v>
       </c>
       <c r="AE118" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="AF118" t="s" s="2">
         <v>43</v>
@@ -15852,10 +15852,10 @@
         <v>45</v>
       </c>
       <c r="AL118" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="AM118" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AN118" t="s" s="2">
         <v>45</v>
@@ -15892,16 +15892,16 @@
         <v>120</v>
       </c>
       <c r="K119" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="L119" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="M119" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="N119" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="O119" t="s" s="2">
         <v>45</v>
@@ -15950,7 +15950,7 @@
         <v>45</v>
       </c>
       <c r="AE119" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AF119" t="s" s="2">
         <v>43</v>
@@ -15971,10 +15971,10 @@
         <v>45</v>
       </c>
       <c r="AL119" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AM119" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AN119" t="s" s="2">
         <v>45</v>
@@ -16014,13 +16014,13 @@
         <v>570</v>
       </c>
       <c r="L120" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="M120" t="s" s="2">
         <v>571</v>
       </c>
       <c r="N120" t="s" s="2">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="O120" t="s" s="2">
         <v>45</v>
@@ -16090,16 +16090,16 @@
         <v>572</v>
       </c>
       <c r="AL120" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="AM120" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="AN120" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO120" t="s" s="2">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="121" hidden="true">
@@ -16133,13 +16133,13 @@
         <v>574</v>
       </c>
       <c r="L121" t="s" s="2">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="M121" t="s" s="2">
         <v>575</v>
       </c>
       <c r="N121" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="O121" t="s" s="2">
         <v>45</v>
@@ -16167,10 +16167,10 @@
         <v>79</v>
       </c>
       <c r="X121" t="s" s="2">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="Y121" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="Z121" t="s" s="2">
         <v>45</v>
@@ -16197,7 +16197,7 @@
         <v>56</v>
       </c>
       <c r="AH121" t="s" s="2">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="AI121" t="s" s="2">
         <v>45</v>
@@ -16212,7 +16212,7 @@
         <v>99</v>
       </c>
       <c r="AM121" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="AN121" t="s" s="2">
         <v>45</v>
@@ -16227,7 +16227,7 @@
       </c>
       <c r="B122" s="2"/>
       <c r="C122" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="D122" s="2"/>
       <c r="E122" t="s" s="2">
@@ -16249,16 +16249,16 @@
         <v>142</v>
       </c>
       <c r="K122" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="L122" t="s" s="2">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="M122" t="s" s="2">
         <v>577</v>
       </c>
       <c r="N122" t="s" s="2">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="O122" t="s" s="2">
         <v>45</v>
@@ -16286,10 +16286,10 @@
         <v>79</v>
       </c>
       <c r="X122" t="s" s="2">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="Y122" t="s" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="Z122" t="s" s="2">
         <v>45</v>
@@ -16325,19 +16325,19 @@
         <v>45</v>
       </c>
       <c r="AK122" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AL122" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="AM122" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AN122" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO122" t="s" s="2">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="123" hidden="true">
@@ -16371,13 +16371,13 @@
         <v>579</v>
       </c>
       <c r="L123" t="s" s="2">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="M123" t="s" s="2">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="N123" t="s" s="2">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="O123" t="s" s="2">
         <v>45</v>
@@ -16447,10 +16447,10 @@
         <v>45</v>
       </c>
       <c r="AL123" t="s" s="2">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="AM123" t="s" s="2">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="AN123" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
Removed demo pages and altered menu layout
</commit_message>
<xml_diff>
--- a/docs/CareConnect-ACVPU-Observation-1.xlsx
+++ b/docs/CareConnect-ACVPU-Observation-1.xlsx
@@ -1979,13 +1979,13 @@
     <col min="2" max="2" width="22.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.6328125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.63671875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1996,22 +1996,22 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="171.48046875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="67.76953125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="72.328125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="242.6875" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="22.03125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Removed base from the name and added support section on main page
</commit_message>
<xml_diff>
--- a/docs/CareConnect-ACVPU-Observation-1.xlsx
+++ b/docs/CareConnect-ACVPU-Observation-1.xlsx
@@ -1979,13 +1979,13 @@
     <col min="2" max="2" width="22.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.6328125" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.63671875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1996,22 +1996,22 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="171.48046875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="67.76953125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="72.328125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="242.6875" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="22.03125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Corrections to support section
</commit_message>
<xml_diff>
--- a/docs/CareConnect-ACVPU-Observation-1.xlsx
+++ b/docs/CareConnect-ACVPU-Observation-1.xlsx
@@ -1979,13 +1979,13 @@
     <col min="2" max="2" width="22.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.63671875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.6328125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1996,22 +1996,22 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="171.48046875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="67.76953125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="72.328125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="242.6875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="22.03125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Verified SNOMED ECL and expanded ValueSets for IG (IgPublisher needs this done). Fixes #11 #13 #14 #15 #16 #17 #19 #23 #22 #21 #29 #30 #31 #32 #37 #41 #42
</commit_message>
<xml_diff>
--- a/docs/CareConnect-ACVPU-Observation-1.xlsx
+++ b/docs/CareConnect-ACVPU-Observation-1.xlsx
@@ -1979,13 +1979,13 @@
     <col min="2" max="2" width="22.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.63671875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.6328125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1996,22 +1996,22 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="171.48046875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="67.76953125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="72.328125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="242.6875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="22.03125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Move of package name to careconnect.base.stu3
</commit_message>
<xml_diff>
--- a/docs/CareConnect-ACVPU-Observation-1.xlsx
+++ b/docs/CareConnect-ACVPU-Observation-1.xlsx
@@ -1979,13 +1979,13 @@
     <col min="2" max="2" width="22.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.63671875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.6328125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1996,22 +1996,22 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="171.48046875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="67.76953125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="72.328125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="242.6875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="22.03125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Replaced English with England context.
</commit_message>
<xml_diff>
--- a/docs/CareConnect-ACVPU-Observation-1.xlsx
+++ b/docs/CareConnect-ACVPU-Observation-1.xlsx
@@ -1979,13 +1979,13 @@
     <col min="2" max="2" width="22.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.63671875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.6328125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1996,22 +1996,22 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="171.48046875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="67.76953125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="72.328125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="242.6875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="22.03125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Errors in file names - probably caused by IgPublisher
</commit_message>
<xml_diff>
--- a/docs/CareConnect-ACVPU-Observation-1.xlsx
+++ b/docs/CareConnect-ACVPU-Observation-1.xlsx
@@ -1979,13 +1979,13 @@
     <col min="2" max="2" width="22.59765625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.6953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.62109375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="11.98828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.7421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="12.74609375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="72.63671875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="72.6328125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1996,22 +1996,22 @@
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.07421875" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="171.48046875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="67.76953125" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.6875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="19.7265625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0390625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="14.984375" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="12.30078125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="40.19140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.21484375" customWidth="true" bestFit="true"/>
+    <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="36" max="36" width="72.328125" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="242.6875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="239.703125" customWidth="true" bestFit="true"/>
     <col min="38" max="38" width="255.0" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="103.87890625" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="22.03125" customWidth="true" bestFit="true"/>

</xml_diff>